<commit_message>
last changes to code
</commit_message>
<xml_diff>
--- a/Project_python/out/LDA/topics_map.xlsx
+++ b/Project_python/out/LDA/topics_map.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.299|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.339|x13:0.000|x14:0.000|x15:0.000|x16:0.362|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.787|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.213|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:1.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.660|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.340|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:1.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:1.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:1.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.455|x5:0.545|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.807|x9:0.000|x10:0.193|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:1.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:1.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.164|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.294|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.359|x13:0.000|x14:0.183|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.127|x4:0.000|x5:0.000|x6:0.873|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:1.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.233|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.767|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:1.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.270|x3:0.000|x4:0.730|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.538|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.462|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>x1:0.818|x2:0.000|x3:0.182|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.517|x12:0.483|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:1.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.312|x10:0.365|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.324|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.770|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.230|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:1.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.207|x8:0.000|x9:0.793|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:1.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>x1:0.356|x2:0.000|x3:0.000|x4:0.000|x5:0.165|x6:0.250|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.228|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:1.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.370|x13:0.000|x14:0.000|x15:0.000|x16:0.630|x17:0.000</t>
+          <t>x1:0.719|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.281|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.177|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.823|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:1.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.378|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.622|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.481|x11:0.000|x12:0.000|x13:0.519|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>x1:1.174|x2:1.447|x3:1.920|x4:1.029|x5:0.935|x6:1.124|x7:1.207|x8:0.807|x9:0.793|x10:1.016|x11:0.767|x12:0.709|x13:0.850|x14:1.000|x15:1.000|x16:1.222|x17:0.000</t>
+          <t>x1:0.719|x2:1.362|x3:1.000|x4:0.455|x5:0.545|x6:1.000|x7:1.081|x8:1.000|x9:1.312|x10:1.467|x11:0.517|x12:0.842|x13:1.732|x14:1.645|x15:1.000|x16:1.324|x17:0.000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All models trained on first time and stored
</commit_message>
<xml_diff>
--- a/Project_python/out/LDA/topics_map.xlsx
+++ b/Project_python/out/LDA/topics_map.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.186|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.628|x13:0.000|x14:0.000|x15:0.000|x16:0.186|x17:0.000</t>
+          <t>x1:0.000|x2:0.186|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.628|x13:0.000|x14:0.000|x15:0.000|x16:0.187|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>x1:0.509|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.295|x9:0.000|x10:0.196|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.509|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.296|x9:0.000|x10:0.196|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.439|x8:0.000|x9:0.220|x10:0.000|x11:0.000|x12:0.000|x13:0.341|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.439|x8:0.000|x9:0.221|x10:0.000|x11:0.000|x12:0.000|x13:0.341|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>x1:1.152|x2:0.681|x3:1.000|x4:0.750|x5:1.000|x6:1.000|x7:1.216|x8:1.475|x9:0.842|x10:1.001|x11:1.107|x12:1.289|x13:1.300|x14:1.000|x15:1.000|x16:1.186|x17:0.000</t>
+          <t>x1:1.151|x2:0.681|x3:1.000|x4:0.750|x5:1.000|x6:1.000|x7:1.216|x8:1.475|x9:0.842|x10:1.002|x11:1.107|x12:1.289|x13:1.300|x14:1.000|x15:1.000|x16:1.187|x17:0.000</t>
         </is>
       </c>
     </row>

</xml_diff>